<commit_message>
Maj soutenance c22 c25
</commit_message>
<xml_diff>
--- a/Referentiel_DFSMarc.xlsx
+++ b/Referentiel_DFSMarc.xlsx
@@ -1741,9 +1741,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="29" width="59.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="29" width="69.57642857142856" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="29" width="29.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="29" width="64.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="29" width="61.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="29" width="21.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="29" width="15.147857142857141" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="29" width="35.14785714285715" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="29" width="51.86214285714286" customWidth="1" bestFit="1"/>
@@ -3315,7 +3315,7 @@
       <c r="Y44" s="4"/>
       <c r="Z44" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="27.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="35.25" customFormat="1" s="1">
       <c r="A45" s="10"/>
       <c r="B45" s="14" t="s">
         <v>107</v>
@@ -3349,7 +3349,7 @@
       <c r="Y45" s="4"/>
       <c r="Z45" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="66" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="35.25" customFormat="1" s="1">
       <c r="A46" s="11"/>
       <c r="B46" s="14" t="s">
         <v>108</v>
@@ -3383,7 +3383,7 @@
       <c r="Y46" s="4"/>
       <c r="Z46" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="30.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A47" s="13"/>
       <c r="B47" s="21" t="s">
         <v>109</v>
@@ -3417,7 +3417,7 @@
       <c r="Y47" s="4"/>
       <c r="Z47" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="42.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A48" s="13"/>
       <c r="B48" s="7" t="s">
         <v>110</v>
@@ -3453,7 +3453,7 @@
       <c r="Y48" s="4"/>
       <c r="Z48" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="35.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A49" s="13"/>
       <c r="B49" s="14" t="s">
         <v>111</v>
@@ -3487,7 +3487,7 @@
       <c r="Y49" s="4"/>
       <c r="Z49" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="36" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A50" s="13"/>
       <c r="B50" s="14" t="s">
         <v>112</v>
@@ -3521,7 +3521,7 @@
       <c r="Y50" s="4"/>
       <c r="Z50" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="50.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A51" s="13"/>
       <c r="B51" s="14" t="s">
         <v>114</v>
@@ -3555,7 +3555,7 @@
       <c r="Y51" s="4"/>
       <c r="Z51" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="36" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A52" s="13"/>
       <c r="B52" s="14" t="s">
         <v>115</v>
@@ -3589,7 +3589,7 @@
       <c r="Y52" s="4"/>
       <c r="Z52" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="36.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="29.25" customFormat="1" s="1">
       <c r="A53" s="13"/>
       <c r="B53" s="21" t="s">
         <v>116</v>
@@ -3623,7 +3623,7 @@
       <c r="Y53" s="4"/>
       <c r="Z53" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="44.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="40.5" customFormat="1" s="1">
       <c r="A54" s="13"/>
       <c r="B54" s="8" t="s">
         <v>117</v>
@@ -3659,7 +3659,7 @@
       <c r="Y54" s="4"/>
       <c r="Z54" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="30" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A55" s="13"/>
       <c r="B55" s="7" t="s">
         <v>118</v>

</xml_diff>